<commit_message>
Updated tests, renamed the style functions from set_style_xyz to style_xyz.
</commit_message>
<xml_diff>
--- a/tests/testthat/xlsx_files/cars.xlsx
+++ b/tests/testthat/xlsx_files/cars.xlsx
@@ -48,9 +48,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="166" formatCode="0.00"/>
-    <numFmt numFmtId="167" formatCode="0"/>
+  <numFmts count="7">
+    <numFmt numFmtId="167" formatCode="#,##0.00"/>
+    <numFmt numFmtId="169" formatCode="#,##0.00"/>
+    <numFmt numFmtId="170" formatCode="#,##0.00"/>
+    <numFmt numFmtId="171" formatCode="#,##0.00"/>
+    <numFmt numFmtId="172" formatCode="#,##0.00"/>
+    <numFmt numFmtId="166" formatCode="#,##0.00"/>
+    <numFmt numFmtId="168" formatCode="0"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -59,11 +64,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <sz val="14"/>
@@ -76,6 +76,11 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <b/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="3">
@@ -146,33 +151,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="170" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="171" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="172" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -467,7 +469,7 @@
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
@@ -478,180 +480,180 @@
       <c r="G1" s="1"/>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
     </row>
     <row r="3">
-      <c r="A3" s="11"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="7" t="s">
+      <c r="A3" s="14"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7" t="s">
+      <c r="E3" s="10"/>
+      <c r="F3" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="7"/>
-      <c r="H3" s="12"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="15"/>
     </row>
     <row r="4">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="12"/>
+      <c r="H4" s="15"/>
     </row>
     <row r="5">
-      <c r="A5" s="10" t="n">
+      <c r="A5" s="12" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="5" t="n">
+      <c r="B5" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="C5" s="13" t="n">
+      <c r="C5" s="16" t="n">
         <v>1</v>
       </c>
       <c r="D5" s="5" t="n">
         <v>91</v>
       </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5" t="n">
+      <c r="E5" s="6"/>
+      <c r="F5" s="7" t="n">
         <v>2.14</v>
       </c>
-      <c r="G5" s="5"/>
-      <c r="H5" s="12"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="15"/>
     </row>
     <row r="6">
-      <c r="A6" s="10" t="n">
+      <c r="A6" s="12" t="n">
         <v>4</v>
       </c>
-      <c r="B6" s="5" t="n">
+      <c r="B6" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="C6" s="13" t="n">
+      <c r="C6" s="16" t="n">
         <v>10</v>
       </c>
       <c r="D6" s="5" t="n">
         <v>81.8</v>
       </c>
-      <c r="E6" s="5" t="n">
+      <c r="E6" s="6" t="n">
         <v>21.8723569831877</v>
       </c>
-      <c r="F6" s="5" t="n">
+      <c r="F6" s="7" t="n">
         <v>2.3003</v>
       </c>
-      <c r="G6" s="5" t="n">
+      <c r="G6" s="8" t="n">
         <v>0.598207331208095</v>
       </c>
-      <c r="H6" s="12"/>
+      <c r="H6" s="15"/>
     </row>
     <row r="7">
-      <c r="A7" s="10" t="n">
+      <c r="A7" s="12" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="5" t="n">
+      <c r="B7" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="C7" s="13" t="n">
+      <c r="C7" s="16" t="n">
         <v>3</v>
       </c>
       <c r="D7" s="5" t="n">
         <v>131.666666666667</v>
       </c>
-      <c r="E7" s="5" t="n">
+      <c r="E7" s="6" t="n">
         <v>37.5277674973257</v>
       </c>
-      <c r="F7" s="5" t="n">
+      <c r="F7" s="7" t="n">
         <v>2.755</v>
       </c>
-      <c r="G7" s="5" t="n">
+      <c r="G7" s="8" t="n">
         <v>0.128160056179763</v>
       </c>
-      <c r="H7" s="12"/>
+      <c r="H7" s="15"/>
     </row>
     <row r="8">
-      <c r="A8" s="10" t="n">
+      <c r="A8" s="12" t="n">
         <v>6</v>
       </c>
-      <c r="B8" s="5" t="n">
+      <c r="B8" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="C8" s="13" t="n">
+      <c r="C8" s="16" t="n">
         <v>4</v>
       </c>
       <c r="D8" s="5" t="n">
         <v>115.25</v>
       </c>
-      <c r="E8" s="5" t="n">
+      <c r="E8" s="6" t="n">
         <v>9.17877987534291</v>
       </c>
-      <c r="F8" s="5" t="n">
+      <c r="F8" s="7" t="n">
         <v>3.38875</v>
       </c>
-      <c r="G8" s="5" t="n">
+      <c r="G8" s="8" t="n">
         <v>0.116216392991695</v>
       </c>
-      <c r="H8" s="12"/>
+      <c r="H8" s="15"/>
     </row>
     <row r="9">
-      <c r="A9" s="9" t="n">
+      <c r="A9" s="13" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="5" t="n">
+      <c r="B9" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="C9" s="13" t="n">
+      <c r="C9" s="16" t="n">
         <v>14</v>
       </c>
       <c r="D9" s="5" t="n">
         <v>209.214285714286</v>
       </c>
-      <c r="E9" s="5" t="n">
+      <c r="E9" s="6" t="n">
         <v>50.9768855182705</v>
       </c>
-      <c r="F9" s="5" t="n">
+      <c r="F9" s="7" t="n">
         <v>3.99921428571429</v>
       </c>
-      <c r="G9" s="5" t="n">
+      <c r="G9" s="8" t="n">
         <v>0.759404744476927</v>
       </c>
-      <c r="H9" s="12"/>
+      <c r="H9" s="15"/>
     </row>
     <row r="10">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>